<commit_message>
v2.1: Full stage logging in main sheet, all columns always filled, TG message sent column, Streamlit deduplication checkbox, analytics by Stage, Google Sheets API optimization
</commit_message>
<xml_diff>
--- a/companies_usa_remote.xlsx
+++ b/companies_usa_remote.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="T1" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
@@ -541,11 +541,11 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>16.02</v>
+        <v>18.76</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>job, manage, resource, team, process, capacity, match, role, company, experience</t>
+          <t>manage, job, team, resource, process, capacity, match, experience, candidates, role</t>
         </is>
       </c>
     </row>
@@ -587,11 +587,11 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>20.08</v>
+        <v>31.11</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>data, com, business, work, res, able, team, skill, analysis, drive</t>
+          <t>data, com, business, work, res, able, team, analysis, skill, skills</t>
         </is>
       </c>
     </row>
@@ -633,11 +633,11 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>40.75</v>
+        <v>64.42</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>management, data, experience, business, work, skills, metrics, portfolio, ability, resource</t>
+          <t>data, management, experience, business, work, skills, ability, metrics, portfolio, able</t>
         </is>
       </c>
     </row>
@@ -679,11 +679,11 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>49.32</v>
+        <v>84.11</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>com, ryder, app, work, job, age, financial, plan, applicant, form</t>
+          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
         </is>
       </c>
     </row>
@@ -725,11 +725,11 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>52.81</v>
+        <v>96.14</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>com, ryder, app, work, job, age, financial, plan, applicant, form</t>
+          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
         </is>
       </c>
     </row>
@@ -771,11 +771,11 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>57.41</v>
+        <v>107.23</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>com, ryder, app, work, job, age, financial, plan, applicant, form</t>
+          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
         </is>
       </c>
     </row>
@@ -817,11 +817,11 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>62.21</v>
+        <v>114.88</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>com, ryder, app, work, job, age, financial, plan, applicant, form</t>
+          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
         </is>
       </c>
     </row>
@@ -863,11 +863,11 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>64.31</v>
+        <v>118.4</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>com, ryder, app, work, job, age, financial, plan, applicant, form</t>
+          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
         </is>
       </c>
     </row>
@@ -909,11 +909,11 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>66.51000000000001</v>
+        <v>121.91</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>com, ryder, app, work, job, age, financial, plan, applicant, form</t>
+          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
         </is>
       </c>
     </row>
@@ -955,11 +955,11 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>68.55</v>
+        <v>125.67</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>com, ryder, app, work, job, age, financial, plan, applicant, form</t>
+          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
         </is>
       </c>
     </row>
@@ -1001,11 +1001,11 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>71.93000000000001</v>
+        <v>135.69</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>com, ryder, app, work, job, age, financial, plan, applicant, form</t>
+          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
         </is>
       </c>
     </row>
@@ -1047,241 +1047,11 @@
         </is>
       </c>
       <c r="K13" t="n">
-        <v>76.61</v>
+        <v>147.77</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>com, work, prime, experience, financial, therapeutics, part, applicant, sit, care</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Jobgether</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Financial Planning &amp; Analysis Senior Analyst - (Remote - USA)</t>
-        </is>
-      </c>
-      <c r="C14" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K14" t="n">
-        <v>102.69</v>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>financial, plan, analysis, planning, job, opportunities, performance, match, strategic, team</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Lensa</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Senior Financial Analyst - REMOTE</t>
-        </is>
-      </c>
-      <c r="C15" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K15" t="n">
-        <v>123.99</v>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>com, ryder, app, work, job, age, financial, plan, applicant, form</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Lensa</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Senior Financial Analyst - REMOTE</t>
-        </is>
-      </c>
-      <c r="C16" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K16" t="n">
-        <v>128.59</v>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>com, ryder, app, work, job, age, financial, plan, applicant, form</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>UNFI</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>FP &amp; A Analyst II- Remote</t>
-        </is>
-      </c>
-      <c r="C17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K17" t="n">
-        <v>149.54</v>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>business, financial, required, remote, work, experience, team, office, able, unfi</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>ClearCaptions, LLC</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Data Analyst (100% Remote)</t>
-        </is>
-      </c>
-      <c r="C18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K18" t="n">
-        <v>188.67</v>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>data, com, business, work, res, able, team, skill, analysis, drive</t>
+          <t>com, work, experience, prime, therapeutics, financial, part, sit, applicant, care</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
streamlit: deduplication strategy selector (first event or prefer TG message sent), user can control which vacancy log to show in analytics
</commit_message>
<xml_diff>
--- a/companies_usa_remote.xlsx
+++ b/companies_usa_remote.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="T1" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
@@ -541,11 +541,11 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>18.76</v>
+        <v>19.66</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>manage, job, team, resource, process, capacity, match, experience, candidates, role</t>
+          <t>manage, job, team, resource, process, match, capacity, role, plan, manager</t>
         </is>
       </c>
     </row>
@@ -587,471 +587,11 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>31.11</v>
+        <v>31.15</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>data, com, business, work, res, able, team, analysis, skill, skills</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>TieTalent</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Business Metrics/Analytics - Remote (Work 8am - 5pm PST Timings)</t>
-        </is>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>64.42</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>data, management, experience, business, work, skills, ability, metrics, portfolio, able</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Lensa</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Senior Financial Analyst - REMOTE</t>
-        </is>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>84.11</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Lensa</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Senior Financial Analyst - REMOTE</t>
-        </is>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>96.14</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Lensa</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Senior Financial Analyst - REMOTE</t>
-        </is>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>107.23</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Lensa</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Senior Financial Analyst - REMOTE</t>
-        </is>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>114.88</v>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Lensa</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Senior Financial Analyst - REMOTE</t>
-        </is>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>118.4</v>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Lensa</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Senior Financial Analyst - REMOTE</t>
-        </is>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>121.91</v>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Lensa</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Senior Financial Analyst - REMOTE</t>
-        </is>
-      </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K11" t="n">
-        <v>125.67</v>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Lensa</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Senior Financial Analyst - REMOTE</t>
-        </is>
-      </c>
-      <c r="C12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>135.69</v>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>com, ryder, app, job, work, age, financial, plan, applicant, form</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Lensa</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Financial Analyst Sr - Remote</t>
-        </is>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K13" t="n">
-        <v>147.77</v>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>com, work, experience, prime, therapeutics, financial, part, sit, applicant, care</t>
+          <t>data, com, business, work, res, able, skill, analysis, team, ability</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: TG message sent deduplication logic in Streamlit, strict string comparison; batch logging for Google Sheets to avoid API quota exceeded
</commit_message>
<xml_diff>
--- a/companies_usa_remote.xlsx
+++ b/companies_usa_remote.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="T1" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
@@ -541,18 +541,18 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>19.66</v>
+        <v>16.75</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>manage, job, team, resource, process, match, capacity, role, plan, manager</t>
+          <t>manage, job, team, process, resource, capacity, match, role, candidates, plan</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Lensa</t>
+          <t>ClearCaptions, LLC</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -587,11 +587,471 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>31.15</v>
+        <v>20.82</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>data, com, business, work, res, able, skill, analysis, team, ability</t>
+          <t>data, com, business, work, res, able, skill, analysis, team, unit</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ride Health</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Workforce Analyst - Fully Remote</t>
+        </is>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>44.67</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>com, age, work, health, ride, time, workforce, manage, any, skill</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>UNFI</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>FP &amp; A Analyst II- Remote</t>
+        </is>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>55.68</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>business, financial, required, experience, remote, work, able, team, unfi, office</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TieTalent</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Business Metrics/Analytics - Remote (Work 8am - 5pm PST Timings)</t>
+        </is>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>65.73</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>data, management, experience, business, work, metrics, skills, ability, portfolio, resource</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kforce Inc</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Finance Manager, Customer Finance - (Remote)</t>
+        </is>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>69.63</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>age, finance, service, financial, kforce, customer, pay, team, act, eligible</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Centene Corporation</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Capacity Planning Analyst II</t>
+        </is>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>85.34</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>per, act, capacity, planning, work, center, contact, perform, experience, standards</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Jobgether</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Workforce Analyst - (Remote - US)</t>
+        </is>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>95.55</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>work, per, staffing, job, workforce, team, time, match, support, candidates</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Jobgether</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Financial Planning &amp; Analysis Senior Analyst - (Remote - USA)</t>
+        </is>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>146.78</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>financial, plan, analysis, planning, job, opportunities, performance, match, candidates, business</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ryder System, Inc.</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Finance Manager - REMOTE</t>
+        </is>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>159.8</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>com, financial, age, ryder, manage, app, work, plan, view, job</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Ryder System, Inc.</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Finance Manager - REMOTE</t>
+        </is>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>162.05</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>com, financial, age, ryder, manage, app, work, plan, view, job</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Ryder System, Inc.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Finance Manager - REMOTE</t>
+        </is>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>164.29</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>com, financial, age, ryder, manage, app, work, plan, view, job</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: all dashboard analytics, charts, and tables now use fully filtered_df (deduplication and TG message sent logic applies everywhere)
</commit_message>
<xml_diff>
--- a/companies_usa_remote.xlsx
+++ b/companies_usa_remote.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="T1" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
@@ -541,11 +541,11 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>16.75</v>
+        <v>16.67</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>manage, job, team, process, resource, capacity, match, role, candidates, plan</t>
+          <t>manage, job, team, process, resource, capacity, match, role, plan, experience</t>
         </is>
       </c>
     </row>
@@ -587,11 +587,11 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>20.82</v>
+        <v>20.61</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>data, com, business, work, res, able, skill, analysis, team, unit</t>
+          <t>data, com, business, work, res, able, team, skill, analysis, unit</t>
         </is>
       </c>
     </row>
@@ -633,11 +633,11 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>44.67</v>
+        <v>46.57</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>com, age, work, health, ride, time, workforce, manage, any, skill</t>
+          <t>age, com, health, work, ride, workforce, time, manage, management, skill</t>
         </is>
       </c>
     </row>
@@ -679,11 +679,11 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>55.68</v>
+        <v>57.33</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>business, financial, required, experience, remote, work, able, team, unfi, office</t>
+          <t>business, financial, required, remote, experience, work, unfi, team, able, office</t>
         </is>
       </c>
     </row>
@@ -725,11 +725,11 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>65.73</v>
+        <v>65.70999999999999</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>data, management, experience, business, work, metrics, skills, ability, portfolio, resource</t>
+          <t>management, data, experience, business, work, metrics, portfolio, skills, ability, able</t>
         </is>
       </c>
     </row>
@@ -771,11 +771,11 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>69.63</v>
+        <v>69.11</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>age, finance, service, financial, kforce, customer, pay, team, act, eligible</t>
+          <t>age, finance, service, customer, kforce, financial, team, pay, act, employee</t>
         </is>
       </c>
     </row>
@@ -817,11 +817,11 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>85.34</v>
+        <v>83.14</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>per, act, capacity, planning, work, center, contact, perform, experience, standards</t>
+          <t>per, act, capacity, planning, work, center, contact, experience, perform, manage</t>
         </is>
       </c>
     </row>
@@ -863,23 +863,23 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>95.55</v>
+        <v>91.70999999999999</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>work, per, staffing, job, workforce, team, time, match, support, candidates</t>
+          <t>work, per, staffing, job, workforce, team, match, time, teams, manage</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Jobgether</t>
+          <t>Ryder System, Inc.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Financial Planning &amp; Analysis Senior Analyst - (Remote - USA)</t>
+          <t>Finance Manager - REMOTE</t>
         </is>
       </c>
       <c r="C10" t="b">
@@ -909,149 +909,11 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>146.78</v>
+        <v>115.76</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>financial, plan, analysis, planning, job, opportunities, performance, match, candidates, business</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Ryder System, Inc.</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Finance Manager - REMOTE</t>
-        </is>
-      </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K11" t="n">
-        <v>159.8</v>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>com, financial, age, ryder, manage, app, work, plan, view, job</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Ryder System, Inc.</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Finance Manager - REMOTE</t>
-        </is>
-      </c>
-      <c r="C12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>162.05</v>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>com, financial, age, ryder, manage, app, work, plan, view, job</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Ryder System, Inc.</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Finance Manager - REMOTE</t>
-        </is>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/</t>
-        </is>
-      </c>
-      <c r="K13" t="n">
-        <v>164.29</v>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>com, financial, age, ryder, manage, app, work, plan, view, job</t>
+          <t>com, age, financial, manage, ryder, app, work, plan, view, job</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
backup: Pre-dashboard improvement - saving current state
Before major Streamlit dashboard refactor based on agent analysis:
- Code-frustration-assessor: CRITICAL RISK (9/10 patterns)
- Business-analyst: Missing core job search workflow
- Streamlit-BI-developer: Complete rewrite needed

Current issues to fix:
- 406 lines with duplicate data loading
- 7 visualizations that don't help job applications
- No export, multi-select, or status tracking
- Hardcoded credentials and mixed languages

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/companies_usa_remote.xlsx
+++ b/companies_usa_remote.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,24 +504,44 @@
           <t>Matched key words</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Search Keyword</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Search Country</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Job Date</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>transformed publish date from description</t>
+        </is>
+      </c>
       <c r="S1" t="inlineStr">
         <is>
           <t>Checked companies:</t>
         </is>
       </c>
       <c r="T1" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>OLIPOP PBC</t>
+          <t>Sayva Solutions</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Demand Planner</t>
+          <t>Financial Planning and Analysis Manager</t>
         </is>
       </c>
       <c r="C2" t="b">
@@ -550,32 +570,52 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4181859450/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=mnOe%2Fh%2BGiFpmCcakY6DtRg%3D%3D&amp;trackingId=c6c1oMkG%2FXoYPjn%2FjI6f2g%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4283551489/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=gpaeOmaMcT6ITyN7ucr0uA%3D%3D&amp;trackingId=gRQQKomMl8RmekK8J5SHDg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>16.47</v>
+        <v>92.34999999999999</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>plan, demand, customer, product, supply, age, experience, olipop, forecast, chain</t>
+          <t>financial, about, erp, present, lead, accounting, experience, years, business, key</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>supply planning, demand planning, forecasting, s&amp;op, remote, fully remote</t>
+          <t>forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>5 days ago</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>2025-04-17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>L&amp;R DISTRIBUTORS</t>
+          <t>Flexton Inc.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Demand Planning Manager</t>
+          <t>Senior Project Manager</t>
         </is>
       </c>
       <c r="C3" t="b">
@@ -604,32 +644,52 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4206243698/?eBP=BUDGET_EXHAUSTED_JOB&amp;refId=mnOe%2Fh%2BGiFpmCcakY6DtRg%3D%3D&amp;trackingId=%2FVBvRZyqnuwWKMrlutLZLw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4286692400/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=gpaeOmaMcT6ITyN7ucr0uA%3D%3D&amp;trackingId=522JsYcu3wxo3pCat60UdA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>19.23</v>
+        <v>115.49</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>per, age, lead, supply, demand, plan, data, forecast, experience, including</t>
+          <t>labor, project, forecasting, lead, manager, integrations, soft, new, est, stakeholder</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>supply planning, demand planning, forecasting, s&amp;op, remote, fully remote, remote position</t>
+          <t>forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>INNBEAUTY PROJECT</t>
+          <t>UGG</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Senior Manager, Demand and Supply Planning</t>
+          <t>Sr. Director, Demand Planning - UGG</t>
         </is>
       </c>
       <c r="C4" t="b">
@@ -658,32 +718,52 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4213042267/?eBP=BUDGET_EXHAUSTED_JOB&amp;refId=mnOe%2Fh%2BGiFpmCcakY6DtRg%3D%3D&amp;trackingId=BwjLTH5e%2BEOXwtc76tlsow%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4281738674/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=9v7sPhR2I6v10s%2B%2B%2FJrI5w%3D%3D&amp;trackingId=MEy9S1l0llvZANwkh8Z2lA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>48.12</v>
+        <v>176.46</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>plan, product, age, demand, manage, planning, forecast, com, supply, sales</t>
+          <t>plan, demand, planning, get, experience, channel, time, work, employee, market</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>supply planning, demand planning, operations planning, forecasting, s&amp;op, sales and operations planning, remote</t>
+          <t>demand planning, forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>2025-04-18</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jobgether</t>
+          <t>The Sage Group</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Capacity Manager ( Remote - US)</t>
+          <t>Regional Operations and Project Manager</t>
         </is>
       </c>
       <c r="C5" t="b">
@@ -712,32 +792,52 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4208600253/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=mnOe%2Fh%2BGiFpmCcakY6DtRg%3D%3D&amp;trackingId=eznQyfbd95m9GU%2FMxTLXfw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4272437959/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=9v7sPhR2I6v10s%2B%2B%2FJrI5w%3D%3D&amp;trackingId=kPWMKiYQwAHja1vEBc9pBg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>51.62</v>
+        <v>179.09</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>manage, job, process, resource, team, capacity, match, experience, role, candidates</t>
+          <t>manage, project, management, community, site, lead, property, experience, operational, housing</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>capacity planning, forecasting, remote, remote work</t>
+          <t>forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>2025-04-01</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>L&amp;R DISTRIBUTORS</t>
+          <t>UGG</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Demand Planning Manager</t>
+          <t>Sr. Director, Demand Planning - UGG</t>
         </is>
       </c>
       <c r="C6" t="b">
@@ -766,32 +866,52 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4207055977/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=FHz%2Fi%2FOQGi72FZaIYC1ehg%3D%3D&amp;trackingId=hZQASPt%2BflRa1TEenLM1lQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4281744004/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=V3DkORIO4Oe1mcf36ER0cQ%3D%3D&amp;trackingId=rDmrWQuKXWGCa5naRgDVVA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>66.31999999999999</v>
+        <v>236.33</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>per, age, lead, supply, demand, plan, data, forecast, experience, including</t>
+          <t>plan, demand, planning, get, experience, channel, time, work, employee, market</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>supply planning, demand planning, forecasting, s&amp;op, remote, fully remote, remote position</t>
+          <t>demand planning, forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>2025-04-18</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hitachi Global Air Power</t>
+          <t>hudsons</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Inventory Control Manager</t>
+          <t>Director of Operations - Launch Stage</t>
         </is>
       </c>
       <c r="C7" t="b">
@@ -820,32 +940,52 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4212396861/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=FHz%2Fi%2FOQGi72FZaIYC1ehg%3D%3D&amp;trackingId=u7iRqIM72QGhSH3QgnaQjA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4285913612/?eBP=BUDGET_EXHAUSTED_JOB&amp;refId=V3DkORIO4Oe1mcf36ER0cQ%3D%3D&amp;trackingId=1z4Tro4WplzpX5b8m5%2FW%2Fg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>68.44</v>
+        <v>239.02</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>inventory, age, manage, order, time, stock, level, demand, levels, work</t>
+          <t>apparel, operations, fashion, operational, build, systems, vendor, medical, mark, brand</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>forecasting, remote</t>
+          <t>inventory planning, remote, remote work</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>3 days ago</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>2025-04-19</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Centene Corporation</t>
+          <t>UGG</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Capacity Planning Analyst II</t>
+          <t>Sr. Director, Demand Planning - UGG</t>
         </is>
       </c>
       <c r="C8" t="b">
@@ -874,32 +1014,52 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4210383348/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=FHz%2Fi%2FOQGi72FZaIYC1ehg%3D%3D&amp;trackingId=mmtHWotn5ca%2BHWlitAaRfw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4281741341/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=5yq3jpTgHwZntidRX8LkfA%3D%3D&amp;trackingId=YKnMvTyiBrMQM5LcKUDpJg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>70.64</v>
+        <v>291</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>per, act, capacity, work, planning, center, contact, experience, perform, other</t>
+          <t>plan, demand, planning, get, experience, channel, time, work, employee, market</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>capacity planning, remote</t>
+          <t>demand planning, forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>2025-04-18</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Carnival Cruise Line</t>
+          <t>Intuvia Technologies</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Shipboard Workforce Planner</t>
+          <t>Supply Chain Analyst</t>
         </is>
       </c>
       <c r="C9" t="b">
@@ -928,32 +1088,52 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4209839267/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=FHz%2Fi%2FOQGi72FZaIYC1ehg%3D%3D&amp;trackingId=N0KvYpIw%2BCx0yCINBXPApQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4286802419/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=f40UJ2fSXPEN5Kq7MfUFDQ%3D%3D&amp;trackingId=UYbadGpz7bXVTgE6AphuXQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>79.18000000000001</v>
+        <v>419.3</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>time, plan, work, employee, part, off, carnival, other, benefits, age</t>
+          <t>supply, manage, chain, management, product, demand, forecast, inventory, sales, skills</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>forecasting, remote</t>
+          <t>demand planning, forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>1 day ago</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>2025-04-21</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Weeks Grp, LLC</t>
+          <t>Insight Global</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Construction Scheduler</t>
+          <t>Capacity &amp; Demand Analyst</t>
         </is>
       </c>
       <c r="C10" t="b">
@@ -982,32 +1162,55 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4209871802/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=FHz%2Fi%2FOQGi72FZaIYC1ehg%3D%3D&amp;trackingId=rsXAcIfE8jIaDW6A%2BF%2FZvQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4283516092/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=KPup3DMmYFpqExxaSUpLNg%3D%3D&amp;trackingId=mzAtXW%2BPUoBZBS0YdM9mQw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>84.06</v>
+        <v>467.32</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>project, schedule, construction, data, center, team, work, experience, projects, weeks</t>
+          <t>experience, portfolio, capacity, plan, management, resource, skills, demand, analyst, project</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>forecasting, remote</t>
-        </is>
-      </c>
+          <t>capacity planning, remote</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Capacity &amp; Demand Analyst
+Capacity &amp; Demand Analyst with verification
+Insight Global
+United States (Remote)
+$40/hr - $45/hr · Vision, 401(k)
+Actively reviewing applicants
+Viewed
+Easy Apply</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Lensa</t>
+          <t>Spiraledge, Inc</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Remote WFM Analyst</t>
+          <t>Planning Analyst</t>
         </is>
       </c>
       <c r="C11" t="b">
@@ -1036,32 +1239,52 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4212681810/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=FHz%2Fi%2FOQGi72FZaIYC1ehg%3D%3D&amp;trackingId=A3xnW8CUgEhi0o65wsZ03w%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4286502904/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=KPup3DMmYFpqExxaSUpLNg%3D%3D&amp;trackingId=KM7KuvpHMYIu1uJ1Pep%2FPA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>90.06999999999999</v>
+        <v>482.95</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>per, act, wfm, 100, experience, 10024, inc, benefit, com, skill</t>
+          <t>planning, per, work, com, team, demand, improve, inventory, sales, experience</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>forecasting, remote</t>
+          <t>inventory planning, demand planning, forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SmartBug Media</t>
+          <t>Dynamic Events, Inc.</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Workforce Planning Manager</t>
+          <t>Event Manager - Logistics &amp; Project Management Focus</t>
         </is>
       </c>
       <c r="C12" t="b">
@@ -1090,32 +1313,52 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4206196423/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=FHz%2Fi%2FOQGi72FZaIYC1ehg%3D%3D&amp;trackingId=uIkHN0lOd%2Bq%2Fc1%2Bvqwp6Ag%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4222843514/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=KPup3DMmYFpqExxaSUpLNg%3D%3D&amp;trackingId=q%2BPDBugsrs%2FU8vwI1Mo4oA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>93.59</v>
+        <v>491.23</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>work, resource, manage, workforce, planning, lead, needs, management, team, ability</t>
+          <t>manage, event, management, ability, project, team, over, time, events, client</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>forecasting, remote, remote work</t>
+          <t>forecasting, remote, work from home, fully remote</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>3 months ago</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>2025-01-22</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Tier4 Group</t>
+          <t>UGG</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SAP IBP Consultant</t>
+          <t>Sr. Director, Demand Planning - UGG</t>
         </is>
       </c>
       <c r="C13" t="b">
@@ -1144,36 +1387,56 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4210731775/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=FHz%2Fi%2FOQGi72FZaIYC1ehg%3D%3D&amp;trackingId=xVcjZnEMAVjrDaYwo%2F34Dw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4281741342/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=KPup3DMmYFpqExxaSUpLNg%3D%3D&amp;trackingId=uIDExrxtiFQgu0fXjRiSEg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>102.12</v>
+        <v>544.4</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>sap, ibp, ability, support, work, understand, week, planning, chain, solution</t>
+          <t>plan, demand, planning, get, experience, channel, time, work, employee, market</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>supply chain planning, remote</t>
+          <t>demand planning, forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>2025-04-18</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Genus PLC</t>
+          <t>Lensa</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Planning, Inventory &amp; Logistics Analyst</t>
+          <t>Sales &amp; Operations Planning (S&amp;OP) Supply Planner</t>
         </is>
       </c>
       <c r="C14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -1198,32 +1461,52 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4208282340/?eBP=BUDGET_EXHAUSTED_JOB&amp;refId=8C%2BVzxtgZgkdbKYPbfA6xQ%3D%3D&amp;trackingId=4sg5Kabc51cCLdnXo5YN3A%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4287293367/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=KPup3DMmYFpqExxaSUpLNg%3D%3D&amp;trackingId=WZMHxUhYbnfnKpULoyWHAw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>117.82</v>
+        <v>558.17</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>plan, work, planning, over, customer, world, logistics, shipment, global, shipments</t>
+          <t>supply, plan, com, job, age, lead, planning, vernova, process, business</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>logistics planning, remote</t>
+          <t>relocation assistance, supply planning, capacity planning, operations planning, forecasting, s&amp;op, sales and operations planning, Relocation Assistance Provided: No, remote, remote position</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>1 day ago</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>2025-04-21</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Casper</t>
+          <t>Binding Minds Inc. (Certified Disability Owned Business Enterprise)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DTC Planner</t>
+          <t>Finance and IT Project Manager</t>
         </is>
       </c>
       <c r="C15" t="b">
@@ -1252,32 +1535,52 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4169965978/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=8C%2BVzxtgZgkdbKYPbfA6xQ%3D%3D&amp;trackingId=oxg9DbxHNtAub6EY5NxPqw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4284517016/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=KPup3DMmYFpqExxaSUpLNg%3D%3D&amp;trackingId=TEJ8xRrj9YChv%2BEPzskw5w%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>120.2</v>
+        <v>566.04</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>com, business, product, report, reporting, casper, including, part, retail, planning</t>
+          <t>project, manage, management, finance, implement, experience, financial, solution, implementation, team</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
           <t>forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>3 days ago</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>2025-04-19</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Cognisol</t>
+          <t>Kate McLeod</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Kinaxis Solutions Consultant - REMOTE</t>
+          <t>Senior Manager, Planning &amp; Operations</t>
         </is>
       </c>
       <c r="C16" t="b">
@@ -1306,32 +1609,52 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4208035188/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=8C%2BVzxtgZgkdbKYPbfA6xQ%3D%3D&amp;trackingId=4SX0aiHRxkWuP3efk2Rfig%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4197615128/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=hZpYSk3tcglwNmk6OuehTQ%3D%3D&amp;trackingId=6D8niZEI%2B%2Bm3iACClrVnVg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>125.28</v>
+        <v>717.75</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>planning, per, supply, kinaxis, functional, experience, chain, rapid, software, process</t>
+          <t>per, plan, age, manage, planning, product, operations, demand, production, supply</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>supply planning, production planning, demand planning, material requirements planning, capacity planning, supply chain planning, s&amp;op, remote</t>
+          <t>production planning, demand planning, supply chain planning, forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>4 months ago</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>2024-12-23</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Tenth Revolution Group</t>
+          <t>Anker Innovations LTD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Syteline Operations Consultant</t>
+          <t>Supply Chain Manager</t>
         </is>
       </c>
       <c r="C17" t="b">
@@ -1360,32 +1683,52 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4210721379/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=8C%2BVzxtgZgkdbKYPbfA6xQ%3D%3D&amp;trackingId=EcCxuhr0moecXR6vY%2BB1eQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4278650679/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=hZpYSk3tcglwNmk6OuehTQ%3D%3D&amp;trackingId=LiQIfQUJQ2wnoNlz6DuX6w%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>132.58</v>
+        <v>746.47</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>syteline, operations, erp, planning, team, implement, consultant, system, business, production</t>
+          <t>com, age, anker, plan, product, planning, demand, work, chain, forecast</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>production planning, remote</t>
+          <t>production planning, demand planning, supply chain planning, forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>1 day ago</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>2025-04-21</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ulteig</t>
+          <t>GlobalSource IT</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Senior Resource Planning Analyst</t>
+          <t>Supply Chain Transformation Project Manager</t>
         </is>
       </c>
       <c r="C18" t="b">
@@ -1414,32 +1757,52 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4186450222/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=8C%2BVzxtgZgkdbKYPbfA6xQ%3D%3D&amp;trackingId=l9x8STVSloCSXyReZ%2BDzFQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4278321337/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=DS3KwMrj3cvtJXyI0Ch06w%3D%3D&amp;trackingId=Xw%2BL%2FxzgjP%2B85BxwArXg%2BQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>137.4</v>
+        <v>803.03</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>rate, plan, work, ulteig, planning, experience, source, resource, utility, skills</t>
+          <t>supply, chain, project, function, able, functional, erp, operations, lead, transformation</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>forecasting, remote</t>
+          <t>supply planning, demand planning, operations planning, s&amp;op, sales and operations planning, remote</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>RSG - Resource Systems Group, Inc.</t>
+          <t>Lantern</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Consultant, Planning Applications</t>
+          <t>Strategy Analyst</t>
         </is>
       </c>
       <c r="C19" t="b">
@@ -1468,15 +1831,15 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4190967336/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=8C%2BVzxtgZgkdbKYPbfA6xQ%3D%3D&amp;trackingId=V5PIj%2B3iFwJ24sJA%2FfvZAQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4266378939/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=xcCHYviEbmOQ6NTfxgeSJQ%3D%3D&amp;trackingId=%2FH%2FTdfesqeCEtbCcd1O1HQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>143.65</v>
+        <v>987.42</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>plan, planning, rsg, develop, win, work, experience, business, transportation, grow</t>
+          <t>care, lantern, team, com, support, high, out, product, drive, opportunities</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -1484,16 +1847,39 @@
           <t>forecasting, remote</t>
         </is>
       </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Strategy Analyst
+Strategy Analyst with verification
+Lantern
+United States (Remote)
+Medical, Dental, Vision, 401(k)
+Actively reviewing applicants
+Viewed
+Easy Apply</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Cognitus</t>
+          <t>Lyra Health</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SAP IBP (no sponsorship provided)</t>
+          <t>Finance Manager - FP&amp;A</t>
         </is>
       </c>
       <c r="C20" t="b">
@@ -1522,32 +1908,52 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4214318188/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=8C%2BVzxtgZgkdbKYPbfA6xQ%3D%3D&amp;trackingId=8vB1w8c8AI%2F1B3wZ6po7uA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4286556685/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=xcCHYviEbmOQ6NTfxgeSJQ%3D%3D&amp;trackingId=UgL9qYbYHK5uCETYHdeKOw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>149.68</v>
+        <v>1008.36</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>sap, experience, ibp, business, planning, work, help, solutions, across, knowledge</t>
+          <t>form, per, format, information, com, financial, lyra, out, inc, health</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>demand planning, supply chain planning, operations planning, remote</t>
+          <t>forecasting, remote, fully remote</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Day One Biopharmaceuticals</t>
+          <t>Insight Global</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Demand Planning, Supply Chain Manager</t>
+          <t>Business Analyst</t>
         </is>
       </c>
       <c r="C21" t="b">
@@ -1576,32 +1982,52 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4211034829/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=DubNOANReKEdyAboqsU8bQ%3D%3D&amp;trackingId=MTgoc0xa09xIwUkVjXLRAw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4286156458/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=gfolC6em6DL3JYEwja3GRw%3D%3D&amp;trackingId=MgpQkZ%2Bi6bgVVMrXBDrO3A%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>168.36</v>
+        <v>1409.53</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>com, one, age, day, supply, able, pharmaceutical, clinical, biopharmaceutical, plan</t>
+          <t>data, business, support, operations, performance, experience, work, operational, ability, team</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>demand planning, forecasting, remote, fully remote</t>
+          <t>forecasting, remote, fully remote</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Iovance Biotherapeutics, Inc.</t>
+          <t>Aquent</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Senior Planner, Clinical Supply Chain</t>
+          <t>Senior Manager Strategic Planning</t>
         </is>
       </c>
       <c r="C22" t="b">
@@ -1630,32 +2056,52 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4192778152/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=DubNOANReKEdyAboqsU8bQ%3D%3D&amp;trackingId=9%2BtEG4jUg31hgmh9PQmIdg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4281390111/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=gfolC6em6DL3JYEwja3GRw%3D%3D&amp;trackingId=1Y%2BBgeLomA8Sp2Ggf453Ew%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>173.18</v>
+        <v>1443.39</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>clinical, com, supply, work, age, able, chain, manage, label, must</t>
+          <t>plan, plannin, rate, planning, levels, product, senior, forecast, manager, low</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>supply planning, remote</t>
+          <t>demand planning, forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Jobs via Dice</t>
+          <t>Alliant Human Capital</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SAP APO PP DS Consultant</t>
+          <t>Production and Supply Chain Manager</t>
         </is>
       </c>
       <c r="C23" t="b">
@@ -1665,7 +2111,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
@@ -1684,32 +2130,52 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4212824220/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=DubNOANReKEdyAboqsU8bQ%3D%3D&amp;trackingId=gEibXMvD6lfOUWjA8RpAKw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4236409944/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=gtDkp%2FpCKTdB5YdrxqZDbw%3D%3D&amp;trackingId=p4vvAt0t1vop6%2FgXzxzYyg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>194.95</v>
+        <v>1493.33</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>sap, planning, apo, scheduling, inc, dice, implement, consultant, career, lead</t>
+          <t>plan, manage, product, planning, production, demand, operations, supply, chain, management</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>sap apo, production planning, demand planning, remote</t>
+          <t>production planning, demand planning, supply chain planning, forecasting, remote</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>2025-04-01</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>TestingXperts</t>
+          <t>NSI Group, LLC</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Remote SAP PMMO Consultant (USC/GC Only)</t>
+          <t>Operations Planning Manager</t>
         </is>
       </c>
       <c r="C24" t="b">
@@ -1738,128 +2204,40 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4212836911/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=DubNOANReKEdyAboqsU8bQ%3D%3D&amp;trackingId=rt60A%2BFc3Q0f5KIubvPO%2BQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4121212510/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=gtDkp%2FpCKTdB5YdrxqZDbw%3D%3D&amp;trackingId=Tj7zALoquCd%2F9tuojCNgWA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>198.76</v>
+        <v>1512.89</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>sap, pmmo, experience, project, work, planning, requirement, requirements, process, gpd</t>
+          <t>manage, plan, product, planning, quality, operations, food, nsi, management, production</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>material requirements planning, capacity planning, remote</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Genus PLC</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Global Demand Planner</t>
-        </is>
-      </c>
-      <c r="C25" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4160574859/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=Vlmd6TJw3svsGRkvVgqL5w%3D%3D&amp;trackingId=renM0fZUUSVsaF0qMTQcPw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
-        </is>
-      </c>
-      <c r="L25" t="n">
-        <v>214.45</v>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>global, demand, genus, com, ability, forecast, any, act, end, genetic</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>supply planning, demand planning, forecasting, s&amp;op, remote</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>ITC Infotech</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>SAP IBP OBP Lead</t>
-        </is>
-      </c>
-      <c r="C26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4177733940/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=FxCS8eHnNjIHvWUnL%2F9nHA%3D%3D&amp;trackingId=CUVwC6rPKO0AwifgOF3U2A%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
-        </is>
-      </c>
-      <c r="L26" t="n">
-        <v>270.41</v>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>sap, ibp, men, planning, business, supply, age, solutions, experience, chain</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>supply planning, demand planning, operations planning, s&amp;op, sales and operations planning, remote</t>
+          <t>production planning, operations planning, forecasting, remote, remote work, remote position</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>remote job, planning manager</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
         </is>
       </c>
     </row>

</xml_diff>